<commit_message>
chore/ fixed role based permissions per page, and other misc fixes
</commit_message>
<xml_diff>
--- a/seed/assignments.xlsx
+++ b/seed/assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerburguillos/AIMS-Project/seed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F366703F-DF25-B84A-B64C-0CD1E02F38D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D122FC8-C7CB-134E-ABB3-2CB3DF381147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D6C39499-9BAE-B647-9BF4-7675D637EA85}"/>
   </bookViews>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42882FD0-5197-784B-B3D7-28926C1A9BA2}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection sqref="A1:G65"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1666,9 +1666,6 @@
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61">
-        <v>11</v>
-      </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>

</xml_diff>